<commit_message>
making progress on excell files
</commit_message>
<xml_diff>
--- a/data/Food_nutrition_Intake/food_table3.xlsx
+++ b/data/Food_nutrition_Intake/food_table3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anikka.martin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20201077\Desktop\DorukGüngör\Eindhoven\Data_Science_AI\Knowledge_Engineering\Knowledge-Engineering-2AMD20-\data\Food_nutrition_Intake\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03C4C403-B338-4E5E-877B-E6AE353A493D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E33C1E-2B83-4A65-98D3-C0BEFC749BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="benchmark out" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Fruits (cups)</t>
   </si>
@@ -59,16 +59,7 @@
     <t>Oils (grams)</t>
   </si>
   <si>
-    <t>Calorie intake levels</t>
-  </si>
-  <si>
-    <t>Recommended food intake per 1,000 calories</t>
-  </si>
-  <si>
     <t>Food group</t>
-  </si>
-  <si>
-    <t>Benchmark food density--recommended food intake per 1,000 calories intake</t>
   </si>
   <si>
     <r>
@@ -478,32 +469,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -650,40 +621,32 @@
     <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="centerContinuous"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -743,9 +706,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -783,9 +746,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -818,26 +781,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -870,26 +816,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1063,9 +992,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1076,226 +1007,201 @@
     <col min="5" max="5" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1400</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D1" s="3">
+        <v>2200</v>
+      </c>
+      <c r="E1" s="3">
+        <v>3000</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.0714300000000001</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.90908999999999995</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.83333000000000002</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="4">
-        <v>1400</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2000</v>
-      </c>
-      <c r="D3" s="4">
-        <v>2200</v>
-      </c>
-      <c r="E3" s="4">
-        <v>3000</v>
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1.0714300000000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.25</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1.36364</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.3333299999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0.10204000000000001</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.12143</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.12987000000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.11905</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.30612</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.39285999999999999</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.38961000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.35714000000000001</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0714300000000001</v>
+        <v>1.7857099999999999</v>
       </c>
       <c r="C6" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.36364</v>
+      </c>
+      <c r="E6" s="1">
         <v>1</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.90908999999999995</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.83333000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>1.0714300000000001</v>
+        <v>3.5714299999999999</v>
       </c>
       <c r="C7" s="1">
-        <v>1.25</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
-        <v>1.36364</v>
+        <v>3.1818200000000001</v>
       </c>
       <c r="E7" s="1">
-        <v>1.3333299999999999</v>
+        <v>3.3333300000000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>0.10204000000000001</v>
+        <v>1.7857099999999999</v>
       </c>
       <c r="C8" s="1">
-        <v>0.12143</v>
+        <v>1.5</v>
       </c>
       <c r="D8" s="1">
-        <v>0.12987000000000001</v>
+        <v>1.59091</v>
       </c>
       <c r="E8" s="1">
-        <v>0.11905</v>
+        <v>1.6666700000000001</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>3</v>
+      <c r="A9" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B9" s="1">
-        <v>0.30612</v>
+        <v>2.8571399999999998</v>
       </c>
       <c r="C9" s="1">
-        <v>0.39285999999999999</v>
+        <v>2.75</v>
       </c>
       <c r="D9" s="1">
-        <v>0.38961000000000001</v>
+        <v>2.7272699999999999</v>
       </c>
       <c r="E9" s="1">
-        <v>0.35714000000000001</v>
+        <v>2.3333300000000001</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1">
-        <v>1.7857099999999999</v>
+        <v>6.25</v>
       </c>
       <c r="C10" s="1">
-        <v>1.5</v>
+        <v>6.25</v>
       </c>
       <c r="D10" s="1">
-        <v>1.36364</v>
+        <v>6.25</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1">
-        <v>3.5714299999999999</v>
-      </c>
-      <c r="C11" s="1">
-        <v>3</v>
-      </c>
-      <c r="D11" s="1">
-        <v>3.1818200000000001</v>
-      </c>
-      <c r="E11" s="1">
-        <v>3.3333300000000001</v>
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4">
+        <v>12.142899999999999</v>
+      </c>
+      <c r="C11" s="4">
+        <v>13.5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>13.181800000000001</v>
+      </c>
+      <c r="E11" s="4">
+        <v>14.666700000000001</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1.7857099999999999</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1.59091</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1.6666700000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1">
-        <v>2.8571399999999998</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2.75</v>
-      </c>
-      <c r="D13" s="1">
-        <v>2.7272699999999999</v>
-      </c>
-      <c r="E13" s="1">
-        <v>2.3333300000000001</v>
+      <c r="A12" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1">
-        <v>6.25</v>
-      </c>
-      <c r="C14" s="1">
-        <v>6.25</v>
-      </c>
-      <c r="D14" s="1">
-        <v>6.25</v>
-      </c>
-      <c r="E14" s="1">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="5">
-        <v>12.142899999999999</v>
-      </c>
-      <c r="C15" s="5">
-        <v>13.5</v>
-      </c>
-      <c r="D15" s="5">
-        <v>13.181800000000001</v>
-      </c>
-      <c r="E15" s="5">
-        <v>14.666700000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>